<commit_message>
Update logic in autopilot
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -254,7 +254,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BM8"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -263,434 +263,329 @@
   <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>TimeStamp</t>
         </is>
       </c>
-      <c r="B1" s="0" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>f1</t>
         </is>
       </c>
-      <c r="C1" s="0" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>f2</t>
         </is>
       </c>
-      <c r="D1" s="0" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>f3</t>
         </is>
       </c>
-      <c r="E1" s="0" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>f4</t>
         </is>
       </c>
-      <c r="F1" s="0" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>f5</t>
         </is>
       </c>
-      <c r="G1" s="0" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>f6</t>
         </is>
       </c>
-      <c r="H1" s="0" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>f7</t>
         </is>
       </c>
-      <c r="I1" s="0" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>f8</t>
         </is>
       </c>
-      <c r="J1" s="0" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>f9</t>
         </is>
       </c>
-      <c r="K1" s="0" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>f10</t>
         </is>
       </c>
-      <c r="L1" s="0" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>f11</t>
         </is>
       </c>
-      <c r="M1" s="0" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>f12</t>
         </is>
       </c>
-      <c r="N1" s="0" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>f13</t>
         </is>
       </c>
-      <c r="O1" s="0" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>f14</t>
         </is>
       </c>
-      <c r="P1" s="0" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>f15</t>
         </is>
       </c>
-      <c r="Q1" s="0" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>f16</t>
         </is>
       </c>
-      <c r="R1" s="0" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>f17</t>
         </is>
       </c>
-      <c r="S1" s="0" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>f18</t>
         </is>
       </c>
-      <c r="T1" s="0" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>f19</t>
         </is>
       </c>
-      <c r="U1" s="0" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>f20</t>
         </is>
       </c>
-      <c r="V1" s="0" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>f21</t>
         </is>
       </c>
-      <c r="W1" s="0" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>f22</t>
         </is>
       </c>
-      <c r="X1" s="0" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>f23</t>
         </is>
       </c>
-      <c r="Y1" s="0" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>f24</t>
         </is>
       </c>
-      <c r="Z1" s="0" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>f25</t>
         </is>
       </c>
-      <c r="AA1" s="0" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>f26</t>
         </is>
       </c>
-      <c r="AB1" s="0" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>f27</t>
         </is>
       </c>
-      <c r="AC1" s="0" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>f28</t>
         </is>
       </c>
-      <c r="AD1" s="0" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>f29</t>
         </is>
       </c>
-      <c r="AE1" s="0" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>f30</t>
         </is>
       </c>
-      <c r="AF1" s="0" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>f31</t>
         </is>
       </c>
-      <c r="AG1" s="0" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>f32</t>
         </is>
       </c>
-      <c r="AH1" s="0" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>f33</t>
         </is>
       </c>
-      <c r="AI1" s="0" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>f34</t>
         </is>
       </c>
-      <c r="AJ1" s="0" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>f35</t>
         </is>
       </c>
-      <c r="AK1" s="0" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>f36</t>
         </is>
       </c>
-      <c r="AL1" s="0" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>f37</t>
         </is>
       </c>
-      <c r="AM1" s="0" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>f38</t>
         </is>
       </c>
-      <c r="AN1" s="0" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>f39</t>
         </is>
       </c>
-      <c r="AO1" s="0" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>f40</t>
         </is>
       </c>
-      <c r="AP1" s="0" t="inlineStr">
+      <c r="AP1" t="inlineStr">
         <is>
           <t>f41</t>
         </is>
       </c>
-      <c r="AQ1" s="0" t="inlineStr">
+      <c r="AQ1" t="inlineStr">
         <is>
           <t>f42</t>
         </is>
       </c>
-      <c r="AR1" s="0" t="inlineStr">
+      <c r="AR1" t="inlineStr">
         <is>
           <t>f43</t>
         </is>
       </c>
-      <c r="AS1" s="0" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>f44</t>
         </is>
       </c>
-      <c r="AT1" s="0" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>f45</t>
         </is>
       </c>
-      <c r="AU1" s="0" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>f46</t>
         </is>
       </c>
-      <c r="AV1" s="0" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>f47</t>
         </is>
       </c>
-      <c r="AW1" s="0" t="inlineStr">
+      <c r="AW1" t="inlineStr">
         <is>
           <t>f48</t>
         </is>
       </c>
-      <c r="AX1" s="0" t="inlineStr">
+      <c r="AX1" t="inlineStr">
         <is>
           <t>f49</t>
         </is>
       </c>
-      <c r="AY1" s="0" t="inlineStr">
+      <c r="AY1" t="inlineStr">
         <is>
           <t>f50</t>
         </is>
       </c>
-      <c r="AZ1" s="0" t="inlineStr">
+      <c r="AZ1" t="inlineStr">
         <is>
           <t>f51</t>
         </is>
       </c>
-      <c r="BA1" s="0" t="inlineStr">
+      <c r="BA1" t="inlineStr">
         <is>
           <t>f52</t>
         </is>
       </c>
-      <c r="BB1" s="0" t="inlineStr">
+      <c r="BB1" t="inlineStr">
         <is>
           <t>f53</t>
         </is>
       </c>
-      <c r="BC1" s="0" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>f54</t>
         </is>
       </c>
-      <c r="BD1" s="0" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>f55</t>
         </is>
       </c>
-      <c r="BE1" s="0" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>f56</t>
         </is>
       </c>
-      <c r="BF1" s="0" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>f57</t>
         </is>
       </c>
-      <c r="BG1" s="0" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>f58</t>
         </is>
       </c>
-      <c r="BH1" s="0" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>f59</t>
         </is>
       </c>
-      <c r="BI1" s="0" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>f60</t>
         </is>
       </c>
-      <c r="BJ1" s="0" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>f61</t>
         </is>
       </c>
-      <c r="BK1" s="0" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>f62</t>
         </is>
       </c>
-      <c r="BL1" s="0" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>f63</t>
         </is>
       </c>
-      <c r="BM1" s="0" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>f64</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>43730.02648918361</v>
-      </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>11,523</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>10,634</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>43730.04239595082</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>11,523</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>10,634</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>43730.04308590291</v>
-      </c>
-      <c r="B4" s="0" t="inlineStr">
-        <is>
-          <t>11,523</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>10,634</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>43730.04377112197</v>
-      </c>
-      <c r="B5" s="0" t="inlineStr">
-        <is>
-          <t>11,523</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>10,634</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>43730.04445703271</v>
-      </c>
-      <c r="B6" s="0" t="inlineStr">
-        <is>
-          <t>11,523</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>10,634</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>43730.04515679704</v>
-      </c>
-      <c r="B7" s="0" t="inlineStr">
-        <is>
-          <t>11,523</t>
-        </is>
-      </c>
-      <c r="C7" s="0" t="inlineStr">
-        <is>
-          <t>10,634</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>43730.04584618493</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>11,523</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>10,634</t>
         </is>
       </c>
     </row>

</xml_diff>